<commit_message>
Archivos Nuevos Agregados - ECD
</commit_message>
<xml_diff>
--- a/TC.xlsx
+++ b/TC.xlsx
@@ -8,46 +8,74 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DGS-HPSTORE.dgs.local\dgs_users$\ecastaneda\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FB7076-C12E-43BF-A692-4CAF5BF2FCE3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50D3FA35-0941-4975-9D41-7C4CE86D254D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1F458B2A-6CB8-45F9-BB67-F3DE57BB21DB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1F458B2A-6CB8-45F9-BB67-F3DE57BB21DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases System Racing" sheetId="1" r:id="rId1"/>
-    <sheet name="Tiempos Estimados de Ejec." sheetId="3" r:id="rId2"/>
-    <sheet name="VSTS_ValidationWS_1" sheetId="2" state="veryHidden" r:id="rId3"/>
+    <sheet name="Tiempos Estimados de Ejec. R" sheetId="3" r:id="rId2"/>
+    <sheet name="Test Cases System Racing Man." sheetId="4" r:id="rId3"/>
+    <sheet name="Tiempos Estimados de Ejec. RM" sheetId="5" r:id="rId4"/>
+    <sheet name="VSTS_ValidationWS_1" sheetId="2" state="veryHidden" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_1" hidden="1">'Test Cases System Racing'!$C$3:$C$61</definedName>
-    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_10015" hidden="1">'Test Cases System Racing'!$D$3:$D$61</definedName>
-    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_2" hidden="1">'Test Cases System Racing'!$E$3:$E$61</definedName>
-    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_80" hidden="1">'Test Cases System Racing'!$F$3:$F$61</definedName>
-    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_n3" hidden="1">'Test Cases System Racing'!$B$3:$B$61</definedName>
-    <definedName name="VSTS_ValidationRange_051dae68cdcb46f898c39c5d5aa86760" hidden="1">VSTS_ValidationWS_1!$AN$1:$AN$4</definedName>
-    <definedName name="VSTS_ValidationRange_079c588775044f7ea1e2948431fd0e51" hidden="1">VSTS_ValidationWS_1!$AC$1:$AC$4</definedName>
+    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_1" hidden="1">'Test Cases System Racing'!$C$3:$C$57</definedName>
+    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_10015" hidden="1">'Test Cases System Racing'!$D$3:$D$57</definedName>
+    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_2" hidden="1">'Test Cases System Racing'!$E$3:$E$57</definedName>
+    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_80" hidden="1">'Test Cases System Racing'!$F$3:$F$57</definedName>
+    <definedName name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_n3" hidden="1">'Test Cases System Racing'!$B$3:$B$57</definedName>
+    <definedName name="VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_1" hidden="1">'Test Cases System Racing Man.'!$C$3:$C$53</definedName>
+    <definedName name="VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_10015" hidden="1">'Test Cases System Racing Man.'!$D$3:$D$53</definedName>
+    <definedName name="VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_2" hidden="1">'Test Cases System Racing Man.'!$E$3:$E$53</definedName>
+    <definedName name="VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_80" hidden="1">'Test Cases System Racing Man.'!$F$3:$F$53</definedName>
+    <definedName name="VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_n3" hidden="1">'Test Cases System Racing Man.'!$B$3:$B$53</definedName>
+    <definedName name="VSTS_ValidationRange_037dbc093a1843749c2c24597284a73d" hidden="1">VSTS_ValidationWS_1!$I$1:$I$3</definedName>
+    <definedName name="VSTS_ValidationRange_0e3d3f5115174032a3dba441fc5644ef" hidden="1">VSTS_ValidationWS_1!$U$1:$U$4</definedName>
+    <definedName name="VSTS_ValidationRange_1179602484694047a3c22b298121b9dc" hidden="1">VSTS_ValidationWS_1!$AL$1:$AL$4</definedName>
+    <definedName name="VSTS_ValidationRange_11fd03ee8e3e49b598ff60260880d513" hidden="1">VSTS_ValidationWS_1!$Z$1</definedName>
     <definedName name="VSTS_ValidationRange_1b4e2847239d46cea48cc11ab227342a" hidden="1">VSTS_ValidationWS_1!$D$1</definedName>
-    <definedName name="VSTS_ValidationRange_2bfd350d28c24916b2dc78c2e7ca0d4e" hidden="1">VSTS_ValidationWS_1!$AB$1:$AB$4</definedName>
-    <definedName name="VSTS_ValidationRange_2e6e4681e5f74f9bb45770ddb2bd401b" hidden="1">VSTS_ValidationWS_1!$AT$1:$AT$7</definedName>
-    <definedName name="VSTS_ValidationRange_311ed9d9e77b4785bf18d417dd32ee2d" hidden="1">VSTS_ValidationWS_1!$AK$1:$AK$2</definedName>
-    <definedName name="VSTS_ValidationRange_3d8e275d8e634d04829ad7733d2df5fd" hidden="1">VSTS_ValidationWS_1!$AF$1:$AF$4</definedName>
-    <definedName name="VSTS_ValidationRange_4249d424b4b7429c9c23a798f00d72a6" hidden="1">VSTS_ValidationWS_1!$AA$1:$AA$7</definedName>
+    <definedName name="VSTS_ValidationRange_1cd0085a2946412abfc188a75d31c359" hidden="1">VSTS_ValidationWS_1!$AS$1:$AS$4</definedName>
+    <definedName name="VSTS_ValidationRange_25d9239b699a41d8915658075572cc0a" hidden="1">VSTS_ValidationWS_1!$F$1:$F$7</definedName>
+    <definedName name="VSTS_ValidationRange_2c296bf079dc4954bbb34575a41e656f" hidden="1">VSTS_ValidationWS_1!$Q$1:$Q$4</definedName>
+    <definedName name="VSTS_ValidationRange_2d52da7bef7343719a3d29786e60cc7c" hidden="1">VSTS_ValidationWS_1!$L$1:$L$4</definedName>
+    <definedName name="VSTS_ValidationRange_3cc8edf977c443bcaf1cebcac7a25941" hidden="1">VSTS_ValidationWS_1!$AT$1:$AT$4</definedName>
+    <definedName name="VSTS_ValidationRange_3daee26388a4476faea870e8804ccc30" hidden="1">VSTS_ValidationWS_1!$AK$1:$AK$11</definedName>
     <definedName name="VSTS_ValidationRange_49648d12eef3485e92f085a855e4bb82" hidden="1">VSTS_ValidationWS_1!$A$1</definedName>
-    <definedName name="VSTS_ValidationRange_592a53c05d004d9bb5e59c8c48ded308" hidden="1">VSTS_ValidationWS_1!$AM$1:$AM$5</definedName>
-    <definedName name="VSTS_ValidationRange_61b0e0e8e95546ccbcf0601f761e114b" hidden="1">VSTS_ValidationWS_1!$AG$1:$AG$4</definedName>
-    <definedName name="VSTS_ValidationRange_65d9ec753c4348a685406e766212f489" hidden="1">VSTS_ValidationWS_1!$AI$1:$AI$4</definedName>
-    <definedName name="VSTS_ValidationRange_6e67d6ee27014a93813216bb733e5fc6" hidden="1">VSTS_ValidationWS_1!$AL$1:$AL$4</definedName>
+    <definedName name="VSTS_ValidationRange_4ad0e884f58c4d749ddbde00dab50ceb" hidden="1">VSTS_ValidationWS_1!$G$1:$G$4</definedName>
+    <definedName name="VSTS_ValidationRange_53afce9541d24c43b5270769a32fae41" hidden="1">VSTS_ValidationWS_1!$AF$1:$AF$2</definedName>
+    <definedName name="VSTS_ValidationRange_5a4e9fe549704a14965277683fcd99dd" hidden="1">VSTS_ValidationWS_1!$AE$1:$AE$4</definedName>
+    <definedName name="VSTS_ValidationRange_61bb1cdc2789430cafcb85fd5a89f906" hidden="1">VSTS_ValidationWS_1!$R$1:$R$5</definedName>
+    <definedName name="VSTS_ValidationRange_6d4dc572ebfb489d8a21f6743ffef6cc" hidden="1">VSTS_ValidationWS_1!$N$1:$N$4</definedName>
+    <definedName name="VSTS_ValidationRange_6fae4de8b93e4f3b8062f3f632c2a0f6" hidden="1">VSTS_ValidationWS_1!$AP$1:$AP$4</definedName>
+    <definedName name="VSTS_ValidationRange_7156d9f52dba46488142bdca035eee88" hidden="1">VSTS_ValidationWS_1!$X$1:$X$11</definedName>
+    <definedName name="VSTS_ValidationRange_71b37ed3f79d41b889989a9fb7bab673" hidden="1">VSTS_ValidationWS_1!$AJ$1:$AJ$7</definedName>
     <definedName name="VSTS_ValidationRange_7505ed56507748d4a8a66d48929e4630" hidden="1">VSTS_ValidationWS_1!$C$1</definedName>
-    <definedName name="VSTS_ValidationRange_7522f74d6bdb4612aca608d81fddc27b" hidden="1">VSTS_ValidationWS_1!$AH$1:$AH$4</definedName>
-    <definedName name="VSTS_ValidationRange_8a0ae347f9e94fe694969787d4da422e" hidden="1">VSTS_ValidationWS_1!$AJ$1:$AJ$4</definedName>
-    <definedName name="VSTS_ValidationRange_a6381ecac7b74ae2b63470d606a2f472" hidden="1">VSTS_ValidationWS_1!$AO$1:$AO$4</definedName>
-    <definedName name="VSTS_ValidationRange_ac79d44db4234907b8fe6e18269df7df" hidden="1">VSTS_ValidationWS_1!$AD$1:$AD$3</definedName>
+    <definedName name="VSTS_ValidationRange_7c3de4aa3c884c2195c80f810579f552" hidden="1">VSTS_ValidationWS_1!$AI$1:$AI$3</definedName>
+    <definedName name="VSTS_ValidationRange_7c8ef6b082514e809423046a98e1b170" hidden="1">VSTS_ValidationWS_1!$Y$1:$Y$7</definedName>
+    <definedName name="VSTS_ValidationRange_7d12462d8915432abaa434774a8d2f83" hidden="1">VSTS_ValidationWS_1!$AG$1:$AG$5</definedName>
+    <definedName name="VSTS_ValidationRange_7f6ccb7df6d7487484423da9a1b89985" hidden="1">VSTS_ValidationWS_1!$AO$1:$AO$4</definedName>
+    <definedName name="VSTS_ValidationRange_8bde6c79bc624873b3b8e906e41f5e24" hidden="1">VSTS_ValidationWS_1!$K$1:$K$4</definedName>
+    <definedName name="VSTS_ValidationRange_90ca0b8ba37a492ba09471ca6924d03d" hidden="1">VSTS_ValidationWS_1!$AB$1:$AB$5</definedName>
+    <definedName name="VSTS_ValidationRange_957aef148d3143d6ad0331666291f2f8" hidden="1">VSTS_ValidationWS_1!$AN$1:$AN$4</definedName>
+    <definedName name="VSTS_ValidationRange_95ca9878f00e4227b038a1809a43bae8" hidden="1">VSTS_ValidationWS_1!$AM$1:$AM$4</definedName>
+    <definedName name="VSTS_ValidationRange_9b31f03ed35845bcacc1dc0598e8dd75" hidden="1">VSTS_ValidationWS_1!$AQ$1:$AQ$4</definedName>
+    <definedName name="VSTS_ValidationRange_a0f80b7860314e51bae3ffc42da4d5a6" hidden="1">VSTS_ValidationWS_1!$P$1:$P$2</definedName>
+    <definedName name="VSTS_ValidationRange_a412f5777bdd44dca0165d52a5a9165a" hidden="1">VSTS_ValidationWS_1!$AC$1:$AC$3</definedName>
+    <definedName name="VSTS_ValidationRange_a4e8c67d0b1a40a1a368d0074f12c4a6" hidden="1">VSTS_ValidationWS_1!$AD$1:$AD$4</definedName>
+    <definedName name="VSTS_ValidationRange_a652f96370304202a9affe34cf549ee0" hidden="1">VSTS_ValidationWS_1!$M$1:$M$4</definedName>
+    <definedName name="VSTS_ValidationRange_af1153d4320842f19f631e7661e3f6d4" hidden="1">VSTS_ValidationWS_1!$V$1:$V$3</definedName>
+    <definedName name="VSTS_ValidationRange_b465c529297f4c188e9cb7417b72090d" hidden="1">VSTS_ValidationWS_1!$H$1:$H$4</definedName>
+    <definedName name="VSTS_ValidationRange_b5d34f075bba4a32913d7b2a065c38b2" hidden="1">VSTS_ValidationWS_1!$AH$1:$AH$4</definedName>
+    <definedName name="VSTS_ValidationRange_bd897986204f4d5480c22d6696a6a77e" hidden="1">VSTS_ValidationWS_1!$O$1:$O$4</definedName>
+    <definedName name="VSTS_ValidationRange_cbd5f08fcae44bb8bc6bd3dcf20de44a" hidden="1">VSTS_ValidationWS_1!$E$1</definedName>
+    <definedName name="VSTS_ValidationRange_d7b1728fd5164ddeba3f31694b2c34da" hidden="1">VSTS_ValidationWS_1!$W$1:$W$4</definedName>
+    <definedName name="VSTS_ValidationRange_d982db6ad88e4ad6a52c5b0e079af2bf" hidden="1">VSTS_ValidationWS_1!$J$1:$J$5</definedName>
     <definedName name="VSTS_ValidationRange_dcf41524871e4033b9032d28760cd1c7" hidden="1">VSTS_ValidationWS_1!$B$1</definedName>
-    <definedName name="VSTS_ValidationRange_eaf84289979a4f58a723ce781b7fc8af" hidden="1">VSTS_ValidationWS_1!$AS$1:$AS$11</definedName>
-    <definedName name="VSTS_ValidationRange_f182d8919b384ded89c2fa38e9fb1545" hidden="1">VSTS_ValidationWS_1!$AP$1:$AP$4</definedName>
-    <definedName name="VSTS_ValidationRange_f67bdafda7e343d081519ea86b82f1d2" hidden="1">VSTS_ValidationWS_1!$AQ$1:$AQ$3</definedName>
-    <definedName name="VSTS_ValidationRange_f7a4cbd5e77f40daa0d8c784ac36bfe1" hidden="1">VSTS_ValidationWS_1!$AE$1:$AE$5</definedName>
-    <definedName name="VSTS_ValidationRange_f7d6fb2bd1e44e9db597ac9f1cc4f4fa" hidden="1">VSTS_ValidationWS_1!$Z$1</definedName>
-    <definedName name="VSTS_ValidationRange_fc48d5dd9c36477580536e998973e60f" hidden="1">VSTS_ValidationWS_1!$AR$1:$AR$4</definedName>
+    <definedName name="VSTS_ValidationRange_f0f5edc53a02485ba02a78e95102f333" hidden="1">VSTS_ValidationWS_1!$AR$1:$AR$4</definedName>
+    <definedName name="VSTS_ValidationRange_f7a1ef42bc874b478a2372554469eb0f" hidden="1">VSTS_ValidationWS_1!$T$1:$T$4</definedName>
+    <definedName name="VSTS_ValidationRange_fb7aa1184590475c9094c76f81db36a3" hidden="1">VSTS_ValidationWS_1!$AA$1:$AA$7</definedName>
+    <definedName name="VSTS_ValidationRange_ffe07137cd7848ccacfd7ce188bc88ff" hidden="1">VSTS_ValidationWS_1!$S$1:$S$4</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -59,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="208">
   <si>
     <t>ID</t>
   </si>
@@ -94,9 +122,6 @@
     <t>all_VSTS_54558f6b_d778_4c34_94c5_d576f6729b82_System.AreaPath</t>
   </si>
   <si>
-    <t>\Sprint 2</t>
-  </si>
-  <si>
     <t>\Sprint 3</t>
   </si>
   <si>
@@ -451,19 +476,43 @@
     <t>\Migracion TC y Ambiente</t>
   </si>
   <si>
-    <t>Verificar que se muestran exitosamente los datos de las OPEN WAGERS para la fecha seleccionada en el reporte WAGER LISTING.</t>
-  </si>
-  <si>
-    <t>Req. Reports Racing</t>
-  </si>
-  <si>
-    <t>Verificar que se muestran exitosamente los datos de las SCORED WAGERS para el rango de fechas seleccionado en el reporte WAGER LISTING.</t>
-  </si>
-  <si>
-    <t>Verificar que se muestran exitosamente los datos de las WAGERS para una RACE de un TRACK indicado en el reporte WAGER ON RACE</t>
-  </si>
-  <si>
-    <t>Verificar que se muestran exitosamente los datos de los resultados de las WAGERS para las RACES en el reporte PROFIT/LOSS BY TRACK</t>
+    <t>Verificar que en la pantalla principal del sistema se muestre la consulta de los datos del BALANCE del PLAYER exitosamente segun las apuestas TO ENTER, OPEN y SCORED.</t>
+  </si>
+  <si>
+    <t>\Test Plans Racing Manager</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos en el reporte WAGER LISTING para las OPEN WAGERS ingresadas para la fecha actual</t>
+  </si>
+  <si>
+    <t>Req. Reports Racing Manager</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos en el reporte WAGER LISTING para el rango de fechas seleccionado para las SCORE WAGERS.</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos RACE en el reporte WAGER ON RACE</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos para las RACES en el reporte PROFIT/LOSS BY TRACK</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos para los TRACKS en el reporte TRACKS LISTING</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos en el reporte TOTE DETAIL</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos en el reporte REBATES DETAIL</t>
+  </si>
+  <si>
+    <t>Verificar que se muestran exitosamente los datos en el reporte POSSIBLE PAST-POST</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar la opcion del Menu About se muestra la informacion de la aplicacion Racing Manager exitosamente.</t>
+  </si>
+  <si>
+    <t>Req. About Racing Manager</t>
   </si>
   <si>
     <r>
@@ -519,7 +568,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Asignadas RACING   </t>
+      <t xml:space="preserve"> Consulta TC Racing   </t>
     </r>
     <r>
       <rPr>
@@ -544,7 +593,274 @@
     </r>
   </si>
   <si>
-    <t>Verificar que en la pantalla principal del sistema se muestre la consulta de los datos del BALANCE del PLAYER exitosamente segun las apuestas TO ENTER, OPEN y SCORED.</t>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_System.AreaPath</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_System.IterationPath</t>
+  </si>
+  <si>
+    <t>Verificar que al ingresar en la ventana Possible Past-Post Tickets se muestran los Tickets de las RACES en Possible Past-Post</t>
+  </si>
+  <si>
+    <t>Req. Tickets Racing Manager</t>
+  </si>
+  <si>
+    <t>Verificar que al cambia la fecha en la ventana Possible Past-Post Tickets se muestran los Possible Past-Post Tickets para la nueva fecha seleccionada</t>
+  </si>
+  <si>
+    <t>***Verificar que al llevar a cabo el VOID TICKET para un registro se anula con exito el Ticket Past Post seleccionado exitosamente.</t>
+  </si>
+  <si>
+    <t>***Verificar que al llevar a cabo el SCORE TICKET para un registro se envia el resultado para la apuesta para el Ticket Past Post seleccionado exitosamente.</t>
+  </si>
+  <si>
+    <t>***Verificar que al ingresar en la ventana Manually Score Tickets se muestran los Tickets de las RACES finalizadas y pendientes de SCORE.</t>
+  </si>
+  <si>
+    <t>***Verificar que al llevar a cabo el SCORE TICKET para un registro de apuesta pendiente de SCORED, se realiza el SCORED para el ticket exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al realizar el proceso de PAY REBATES en la ventana PAY REBATES se realiza el pago de los REBATES exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que se muestra las opciones del menu Tote Tickets exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar la opcion Exit del Menu File se cierra la aplicacion Racing Manager exitosamente.</t>
+  </si>
+  <si>
+    <t>Req. File Racing Manager</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar la opcion Close, SI HAY ventanas abiertas en el RACING MANAGER se cierran cada una de ellas.</t>
+  </si>
+  <si>
+    <t>Verificar que al abrir la ventana de LIMIT SETS se muestran la pantalla exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar NEW en la ventana de LIMIT SETS se crea un nuevo conjunto de LIMIT SETS exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar Delete en la ventana de LIMIT SETS se valide que se tenga seleccionado un conjunto de LIMIT SET</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar Delete se elimine el limit set seleccionado exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar Delete en la ventana de LIMIT SETS se valide si el LIMIT SET esta asignado aun conjunto de LIMITS.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar Clone en la ventana de LIMIT SETS se crea un nuevo conjunto de LIMIT SETS con la misma informacion del LIMIT SET seleccionado exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al abrir la ventana de LIMITS se muestran la pantalla exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al abrir la ventana de TRACKS se muestran la pantalla exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al seleccionar alguno de los TRACKS en la ventana de TRACKS se muestre la informacion del mismo en los campos de la pantalla exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al realizar cambios a la informacion de alguno de los TRACKS y presionar el boton CANCELAR se deshacen los cambios ingresados y se muestran pantalla exitosamente los datos originales para el tracks seleccionado.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar el boton NUEVO exitosamente se limpian los campos en la pantalla para ingresar los datos del nuevo TRACK, y al presionar GUARDAR exitosamente SE guardan los datos y se muestra el nuevo TRACK en el listado.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar el boton NUEVO exitosamente se limpian los campos en la pantalla para ingresar los datos del nuevo TRACK, y al presionar CANCELAR exitosamente NO SE guardan los datos y NO SE muestra el nuevo TRACK en el listado.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar Eliminar para alguno de los TRACKS se muestre un mensaje de validacion para eliminar el registro del track; y se elimina o no el registro exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al abrir la ventana de PROFILE TRACKS se muestran la pantalla exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al se permite pasar tracks de habilitado a deshabilitado (y viceversa) en la ventana de PROFILE TRACKS exitosamente en cada uno de los tab's.</t>
+  </si>
+  <si>
+    <t>VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_E4-CA-08-0D-C5-01-AB-82-96-6F-B8-39-E9-3E-EA-3F-57-42-86-2A</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Bug_System.State</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Epic_System.State</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Feature_System.State</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Impediment_System.State</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Product Backlog Item_System.State</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Task_System.State</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Test Case_System.State</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_System.WorkItemType</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_System.State</t>
+  </si>
+  <si>
+    <t>VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_A9-74-3C-60-20-83-BF-D2-70-44-DA-6E-AF-8C-55-96-9A-24-CE-B3</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Bug_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Epic_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Feature_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Impediment_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Product Backlog Item_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Task_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Test Case_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>all_VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc_Microsoft.VSTS.Common.Priority</t>
+  </si>
+  <si>
+    <t>Verificar que al ingresar a la pantalla Open del menu Races se muestra exitosamente.</t>
+  </si>
+  <si>
+    <t>Req. Races Racing Manager</t>
+  </si>
+  <si>
+    <t>Verificar que al ingresar a la pantalla Console del menu Races se muestra exitosamente segun la opcion utilizada (Today, Yesterday o Choose Date)</t>
+  </si>
+  <si>
+    <t>Verificar que al modificar los datos de una RACE en la pantalla Open se guardan y se refresca la consulta de los datos exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al modificar los datos de una RACE en la pantalla Open y refrescar los datos se realiza la consulta de los datos exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al seleccionar un TRACK ACTIVE en la pantalla Console se muestra las RACES del dia para el TRACK seleccionado exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al seleccionar una de las UPCOMING RACES en la pantalla Console se muestra las RACES del dia y los datos de los ENTRIES para la RACE seleccionada exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que se actualizan los MTP y ESTADO de la RACE en la pantalla Console exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar View Possible Past-Post se muestra la pantalla de los Past-Post Tickets para la RACE seleccionada exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al presionar Set Status Complete para una RACE se modifica el estado de la RACE a estado COMPLETE exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al pasar una RACE a estado OFF se muestre en la pantalla Console los datos de los ENTRIES para la RACE, el estado OFF y la hora OFF TIME exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que al pasar una RACE a Estado COMPLETE se muestre en la pantalla Console los resultados en cada una de las apuestas, el tiempo Post-Time y el estado Complete; exitosamente.</t>
+  </si>
+  <si>
+    <t>Verificar que se identifiquen los ENTRIES en SCRATCHED en la pantalla de la consola de manera exitosa.</t>
+  </si>
+  <si>
+    <t>Verificar que al completarse una RACE y se ingresen los resultados SI existen apuestas ingresadas se ingresa el monto perdido/ganado por cada una de las apuestas (se realiza el SCORE de las apuestas)</t>
+  </si>
+  <si>
+    <t>Verificar que al completarse una RACE, se ingresen los resultados, se realiza UNSCORE TICKETS y se realice el SCORE TICKETS nuevamente; SI existen apuestas ingresadas se vuelvan a mostrar las apuestas en la consulta de HISTORY exitosamente</t>
+  </si>
+  <si>
+    <t>Verificar que al completarse una RACE, se ingresen los resultados, se realiza UNSCORE TICKETS; SI existen apuestas se vuelvan a mostrar las apuestas en la consulta de OPEN BETS exitosamente</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Proyecto: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">QA Department   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Servidor:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 192.168.30.122\DGS QA   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Consulta:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Consulta TC Racing Manager   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Tipo de lista:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Plano    </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -898,7 +1214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -968,6 +1284,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1037,12 +1354,38 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1080,14 +1423,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B723EAEB-7FFC-4C0C-8B07-2CC2F7C05F36}" name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82" displayName="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82" ref="B3:F61" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="B3:F61" xr:uid="{1796E27B-4286-4DEA-A81E-0EF147E6AD63}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B723EAEB-7FFC-4C0C-8B07-2CC2F7C05F36}" name="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82" displayName="VSTS_54558f6b_d778_4c34_94c5_d576f6729b82" ref="B3:F57" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="B3:F57" xr:uid="{235540F1-0280-42A6-81FF-B4C710228380}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{C5DA0111-CD93-483A-9932-365A9D7F08BB}" name="ID" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{B25019E4-8827-41DF-9CA9-2E835EE4CF4E}" name="Title" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{A60A8A61-EE15-4B8E-A82F-E204425179A9}" name="Priority" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{6A71F40A-1D5F-43E2-9CB1-99B363BA43C7}" name="State" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{946738A5-A5D8-4AEE-8511-4768E726B4AC}" name="Tags" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C5DA0111-CD93-483A-9932-365A9D7F08BB}" name="ID" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B25019E4-8827-41DF-9CA9-2E835EE4CF4E}" name="Title" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{A60A8A61-EE15-4B8E-A82F-E204425179A9}" name="Priority" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{6A71F40A-1D5F-43E2-9CB1-99B363BA43C7}" name="State" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{946738A5-A5D8-4AEE-8511-4768E726B4AC}" name="Tags" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{132CEFBC-2F9B-4036-85D9-6523F9B6E2BB}" name="VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc" displayName="VSTS_cd8cbdcb_e314_4fa1_af74_79c4f0b05edc" ref="B3:F53" totalsRowShown="0">
+  <autoFilter ref="B3:F53" xr:uid="{C23AFA75-BC09-4EE2-A875-16838CC5D992}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{D10AFDCD-BCEA-4329-B17E-E021B454A66A}" name="ID" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C79FA00B-1303-4C3E-97ED-1119AEB2CB53}" name="Title" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{07F4A806-96E1-45CB-9E22-F7631AD4C861}" name="Priority" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{6EC59BF3-CA7A-4C2C-A25D-8BAC5ACA28EF}" name="State" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{129B83FF-1B98-4E47-BA71-4D06222151CD}" name="Tags" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1390,10 +1747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521722B8-FC1C-4685-B44D-5D4D37344C53}">
-  <dimension ref="B2:F61"/>
+  <dimension ref="B2:F57"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B61" sqref="B4:B61"/>
+    <sheetView topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1409,7 +1766,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="23" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="19"/>
@@ -1424,7 +1781,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" s="20" t="s">
         <v>2</v>
@@ -1438,16 +1795,16 @@
         <v>32</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D4" s="21">
         <v>2</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1455,16 +1812,16 @@
         <v>37</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="21">
         <v>4</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1472,16 +1829,16 @@
         <v>38</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="21">
         <v>4</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -1489,16 +1846,16 @@
         <v>39</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" s="21">
         <v>2</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1506,16 +1863,16 @@
         <v>40</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="21">
         <v>4</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1523,16 +1880,16 @@
         <v>41</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="21">
         <v>4</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1540,16 +1897,16 @@
         <v>43</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="21">
         <v>2</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1557,16 +1914,16 @@
         <v>44</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="21">
+        <v>3</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="22" t="s">
         <v>68</v>
-      </c>
-      <c r="D11" s="21">
-        <v>3</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1574,16 +1931,16 @@
         <v>45</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D12" s="21">
         <v>3</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -1591,16 +1948,16 @@
         <v>46</v>
       </c>
       <c r="C13" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="21">
+        <v>3</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="22" t="s">
         <v>65</v>
-      </c>
-      <c r="D13" s="21">
-        <v>3</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1608,16 +1965,16 @@
         <v>50</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D14" s="21">
         <v>3</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -1625,16 +1982,16 @@
         <v>51</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D15" s="21">
         <v>3</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -1642,16 +1999,16 @@
         <v>52</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="21">
         <v>3</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1659,16 +2016,16 @@
         <v>53</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D17" s="21">
         <v>3</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -1676,16 +2033,16 @@
         <v>54</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D18" s="21">
         <v>3</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F18" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -1693,16 +2050,16 @@
         <v>55</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="21">
         <v>3</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -1710,16 +2067,16 @@
         <v>56</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D20" s="21">
         <v>1</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1727,16 +2084,16 @@
         <v>57</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D21" s="21">
         <v>4</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -1744,16 +2101,16 @@
         <v>58</v>
       </c>
       <c r="C22" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="21">
         <v>4</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F22" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -1761,16 +2118,16 @@
         <v>59</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="21">
         <v>2</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F23" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -1778,16 +2135,16 @@
         <v>62</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="21">
         <v>3</v>
       </c>
       <c r="E24" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F24" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -1795,16 +2152,16 @@
         <v>63</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" s="21">
         <v>3</v>
       </c>
       <c r="E25" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F25" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -1812,16 +2169,16 @@
         <v>64</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D26" s="21">
         <v>2</v>
       </c>
       <c r="E26" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
@@ -1829,16 +2186,16 @@
         <v>65</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D27" s="21">
         <v>2</v>
       </c>
       <c r="E27" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F27" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
@@ -1846,16 +2203,16 @@
         <v>66</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D28" s="21">
         <v>2</v>
       </c>
       <c r="E28" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F28" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
@@ -1863,16 +2220,16 @@
         <v>67</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="21">
         <v>1</v>
       </c>
       <c r="E29" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
@@ -1880,16 +2237,16 @@
         <v>68</v>
       </c>
       <c r="C30" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D30" s="21">
         <v>1</v>
       </c>
       <c r="E30" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
@@ -1897,16 +2254,16 @@
         <v>69</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D31" s="21">
         <v>1</v>
       </c>
       <c r="E31" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F31" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
@@ -1914,16 +2271,16 @@
         <v>70</v>
       </c>
       <c r="C32" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D32" s="21">
         <v>1</v>
       </c>
       <c r="E32" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
@@ -1931,16 +2288,16 @@
         <v>71</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D33" s="21">
         <v>1</v>
       </c>
       <c r="E33" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F33" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
@@ -1948,16 +2305,16 @@
         <v>72</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D34" s="21">
         <v>1</v>
       </c>
       <c r="E34" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F34" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
@@ -1965,16 +2322,16 @@
         <v>73</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="21">
         <v>1</v>
       </c>
       <c r="E35" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
@@ -1982,16 +2339,16 @@
         <v>74</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D36" s="21">
         <v>1</v>
       </c>
       <c r="E36" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
@@ -1999,16 +2356,16 @@
         <v>75</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="21">
         <v>1</v>
       </c>
       <c r="E37" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F37" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
@@ -2016,16 +2373,16 @@
         <v>76</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" s="21">
         <v>1</v>
       </c>
       <c r="E38" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F38" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
@@ -2033,16 +2390,16 @@
         <v>77</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D39" s="21">
         <v>1</v>
       </c>
       <c r="E39" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F39" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
@@ -2050,16 +2407,16 @@
         <v>78</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D40" s="21">
         <v>1</v>
       </c>
       <c r="E40" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F40" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
@@ -2067,16 +2424,16 @@
         <v>79</v>
       </c>
       <c r="C41" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" s="21">
         <v>4</v>
       </c>
       <c r="E41" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F41" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
@@ -2084,16 +2441,16 @@
         <v>80</v>
       </c>
       <c r="C42" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="21">
         <v>2</v>
       </c>
       <c r="E42" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F42" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
@@ -2101,16 +2458,16 @@
         <v>81</v>
       </c>
       <c r="C43" s="17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" s="21">
         <v>2</v>
       </c>
       <c r="E43" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F43" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="44" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -2118,16 +2475,16 @@
         <v>82</v>
       </c>
       <c r="C44" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D44" s="21">
         <v>2</v>
       </c>
       <c r="E44" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F44" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="45" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -2135,16 +2492,16 @@
         <v>83</v>
       </c>
       <c r="C45" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D45" s="21">
         <v>2</v>
       </c>
       <c r="E45" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F45" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
@@ -2152,16 +2509,16 @@
         <v>84</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D46" s="21">
         <v>3</v>
       </c>
       <c r="E46" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F46" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
@@ -2169,16 +2526,16 @@
         <v>85</v>
       </c>
       <c r="C47" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D47" s="21">
         <v>3</v>
       </c>
       <c r="E47" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F47" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
@@ -2186,16 +2543,16 @@
         <v>86</v>
       </c>
       <c r="C48" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D48" s="21">
         <v>3</v>
       </c>
       <c r="E48" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -2203,16 +2560,16 @@
         <v>87</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D49" s="21">
         <v>3</v>
       </c>
       <c r="E49" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F49" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -2220,16 +2577,16 @@
         <v>88</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D50" s="21">
         <v>1</v>
       </c>
       <c r="E50" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F50" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
@@ -2237,16 +2594,16 @@
         <v>89</v>
       </c>
       <c r="C51" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D51" s="21">
         <v>1</v>
       </c>
       <c r="E51" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F51" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
@@ -2254,16 +2611,16 @@
         <v>90</v>
       </c>
       <c r="C52" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D52" s="21">
         <v>1</v>
       </c>
       <c r="E52" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F52" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
@@ -2271,16 +2628,16 @@
         <v>91</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D53" s="21">
         <v>2</v>
       </c>
       <c r="E53" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F53" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="54" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -2288,16 +2645,16 @@
         <v>92</v>
       </c>
       <c r="C54" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D54" s="21">
         <v>2</v>
       </c>
       <c r="E54" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="22" t="s">
         <v>19</v>
-      </c>
-      <c r="F54" s="22" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
@@ -2305,16 +2662,16 @@
         <v>93</v>
       </c>
       <c r="C55" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D55" s="21">
         <v>1</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F55" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
@@ -2322,134 +2679,86 @@
         <v>94</v>
       </c>
       <c r="C56" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="21">
+        <v>3</v>
+      </c>
+      <c r="E56" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="21">
-        <v>3</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>22</v>
-      </c>
       <c r="F56" s="22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="21">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D57" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E57" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F57" s="22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="21">
-        <v>102</v>
-      </c>
-      <c r="C58" s="17" t="s">
-        <v>132</v>
-      </c>
-      <c r="D58" s="21">
-        <v>2</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" s="22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="21">
-        <v>103</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="D59" s="21">
-        <v>2</v>
-      </c>
-      <c r="E59" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" s="22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="21">
-        <v>104</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="D60" s="21">
-        <v>2</v>
-      </c>
-      <c r="E60" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="22" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="21">
-        <v>106</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D61" s="21">
-        <v>3</v>
-      </c>
-      <c r="E61" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
-    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B3" xr:uid="{5E5E5B24-3A39-4E7C-B3D8-36F8659D808B}">
+  <dataValidations count="16">
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B3" xr:uid="{87E3EA2C-A19D-4974-8797-A2A7787E2EB2}">
       <formula1>"ID"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="C3" xr:uid="{F394EE00-7284-4F1A-9CA1-F454CC2FB8AF}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="C3" xr:uid="{18FC5D09-EAA4-4A35-B0D3-8C8C1E7DDA49}">
       <formula1>"Title"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="D3" xr:uid="{BDC8E8F8-FBEB-47AF-8B1E-B5E64205FE7D}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="D3" xr:uid="{001E3688-6ADB-4984-8C13-D071FE9EFA17}">
       <formula1>"Priority"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="E3" xr:uid="{43FEDD24-5F6C-4DBE-ADBF-48C7B556151A}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="E3" xr:uid="{BAD0BDE9-1214-4EFC-A247-226A8C7FB30F}">
       <formula1>"State"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="F3" xr:uid="{283E22E5-FA9E-4434-978F-0088F2770B21}">
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="F3" xr:uid="{6242684C-BEF9-4F1A-8008-83F4F3595065}">
       <formula1>"Tags"</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B61" xr:uid="{3859EC84-C88C-4643-9FCD-BE19B0C608CA}">
-      <formula1>"106"</formula1>
+    <dataValidation type="list" operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B6" xr:uid="{59F7D8AB-7CD5-4D69-A43B-FED36ED56A58}">
+      <formula1>"38"</formula1>
     </dataValidation>
-    <dataValidation type="textLength" showInputMessage="1" sqref="C61" xr:uid="{CB7F244A-C64E-41F3-9DF7-5007DBDC9505}">
+    <dataValidation type="textLength" showInputMessage="1" sqref="C6 C11" xr:uid="{75811DED-67CA-40AD-93DB-116B3032C472}">
       <formula1>1</formula1>
       <formula2>255</formula2>
     </dataValidation>
-    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="D61" xr:uid="{B1199D93-CC71-4AA1-84F6-1F5535BC9A8B}">
-      <formula1>VSTS_ValidationRange_079c588775044f7ea1e2948431fd0e51</formula1>
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="D6 D11" xr:uid="{93B6B569-2F1B-4812-A408-9D50FCD443BF}">
+      <formula1>VSTS_ValidationRange_b465c529297f4c188e9cb7417b72090d</formula1>
     </dataValidation>
-    <dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="E61" xr:uid="{BDED996B-2E13-4A50-A178-BEC55ECC08AC}">
-      <formula1>VSTS_ValidationRange_ac79d44db4234907b8fe6e18269df7df</formula1>
+    <dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="E6 E11" xr:uid="{FAFD15D8-70BE-4698-A986-39CE6FD60D93}">
+      <formula1>VSTS_ValidationRange_037dbc093a1843749c2c24597284a73d</formula1>
     </dataValidation>
-    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" sqref="F61" xr:uid="{6CF07573-F202-49A3-930A-8D765DF9F58F}">
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" sqref="F6 F11" xr:uid="{6B9FA4B3-0CBF-48FE-9E16-FAECF78DA9FA}">
+      <formula1>0</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B11" xr:uid="{C5F78EB5-AF1B-4EF8-BC52-67F3D0A61542}">
+      <formula1>"44"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B4" xr:uid="{D7F6704E-13FC-4D29-8DE2-AC88B1A16613}">
+      <formula1>"32"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" showInputMessage="1" sqref="C4" xr:uid="{E38DFA10-45BF-438A-BBA2-429EFE125C65}">
+      <formula1>1</formula1>
+      <formula2>255</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="D4" xr:uid="{99BBBE76-9781-4098-9843-4221F0EEE42A}">
+      <formula1>VSTS_ValidationRange_b465c529297f4c188e9cb7417b72090d</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="E4" xr:uid="{18FD1BAC-C203-4554-97B4-2CE4920B5591}">
+      <formula1>VSTS_ValidationRange_037dbc093a1843749c2c24597284a73d</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" sqref="F4" xr:uid="{129F5356-BC16-4993-BDA5-69E41A40E4E8}">
       <formula1>0</formula1>
       <formula2>32767</formula2>
     </dataValidation>
@@ -2466,190 +2775,190 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8228A6C-BCF9-4417-8396-B1350FE2E6C2}">
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="47"/>
-      <c r="H2" s="36" t="s">
-        <v>128</v>
-      </c>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="H2" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="27"/>
       <c r="H3" s="14">
         <v>1</v>
       </c>
-      <c r="I3" s="29">
+      <c r="I3" s="30">
         <v>40</v>
       </c>
-      <c r="J3" s="30"/>
+      <c r="J3" s="31"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C4" s="27">
-        <f>COUNTIF('Test Cases System Racing'!D4:D105,1)</f>
+        <v>116</v>
+      </c>
+      <c r="C4" s="28">
+        <f>COUNTIF('Test Cases System Racing'!D4:D101,1)</f>
         <v>17</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29">
+      <c r="D4" s="29"/>
+      <c r="E4" s="30">
         <f>C4*I3</f>
         <v>680</v>
       </c>
-      <c r="F4" s="30"/>
+      <c r="F4" s="31"/>
       <c r="H4" s="14">
         <v>2</v>
       </c>
-      <c r="I4" s="29">
+      <c r="I4" s="30">
         <v>30</v>
       </c>
-      <c r="J4" s="30"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="C5" s="27">
-        <f>COUNTIF('Test Cases System Racing'!D4:D105,2)</f>
-        <v>17</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29">
+        <v>117</v>
+      </c>
+      <c r="C5" s="28">
+        <f>COUNTIF('Test Cases System Racing'!D4:D101,2)</f>
+        <v>13</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30">
         <f>C5*I4</f>
-        <v>510</v>
-      </c>
-      <c r="F5" s="30"/>
+        <v>390</v>
+      </c>
+      <c r="F5" s="31"/>
       <c r="H5" s="14">
         <v>3</v>
       </c>
-      <c r="I5" s="29">
+      <c r="I5" s="30">
         <v>15</v>
       </c>
-      <c r="J5" s="30"/>
+      <c r="J5" s="31"/>
     </row>
     <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C6" s="27">
-        <f>COUNTIF('Test Cases System Racing'!D4:D105,3)</f>
+        <v>118</v>
+      </c>
+      <c r="C6" s="28">
+        <f>COUNTIF('Test Cases System Racing'!D4:D101,3)</f>
         <v>17</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="29">
+      <c r="D6" s="29"/>
+      <c r="E6" s="30">
         <f>C6*I5</f>
         <v>255</v>
       </c>
-      <c r="F6" s="30"/>
+      <c r="F6" s="31"/>
       <c r="H6" s="15">
         <v>4</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I6" s="40">
         <v>5</v>
       </c>
-      <c r="J6" s="40"/>
+      <c r="J6" s="41"/>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="C7" s="27">
-        <f>COUNTIF('Test Cases System Racing'!D4:D105,4)</f>
+        <v>119</v>
+      </c>
+      <c r="C7" s="28">
+        <f>COUNTIF('Test Cases System Racing'!D4:D101,4)</f>
         <v>7</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="39">
+      <c r="D7" s="29"/>
+      <c r="E7" s="40">
         <f>C7*I6</f>
         <v>35</v>
       </c>
-      <c r="F7" s="40"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="43"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
     </row>
     <row r="9" spans="2:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="45">
+        <f>SUM(C4:C7)</f>
+        <v>54</v>
+      </c>
+      <c r="D9" s="45"/>
+      <c r="E9" s="9" t="s">
         <v>121</v>
-      </c>
-      <c r="C9" s="44">
-        <f>SUM(C4:C7)</f>
-        <v>58</v>
-      </c>
-      <c r="D9" s="44"/>
-      <c r="E9" s="9" t="s">
-        <v>122</v>
       </c>
       <c r="F9" s="10">
         <f>SUM(E4:F7)</f>
-        <v>1480</v>
+        <v>1360</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="32">
+        <f>F9/60</f>
+        <v>22.666666666666668</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="12" t="s">
         <v>123</v>
-      </c>
-      <c r="C10" s="31">
-        <f>F9/60</f>
-        <v>24.666666666666668</v>
-      </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="12" t="s">
-        <v>124</v>
       </c>
       <c r="F10" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="35">
+        <f>C10/F10</f>
+        <v>4.5333333333333332</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="C11" s="34">
-        <f>C10/F10</f>
-        <v>4.9333333333333336</v>
-      </c>
-      <c r="D11" s="34"/>
-      <c r="E11" s="12" t="s">
-        <v>126</v>
       </c>
       <c r="F11" s="5">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="33"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F12" s="7">
         <f>F11*F10</f>
@@ -2685,6 +2994,1187 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F40836E-8757-4652-A6D3-75C200CEDAAA}">
+  <dimension ref="B2:F53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.140625" style="22" customWidth="1"/>
+    <col min="3" max="3" width="100.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="22" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="22" customWidth="1"/>
+    <col min="6" max="6" width="32" style="22" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
+    <col min="8" max="8" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="21">
+        <v>101</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="21">
+        <v>3</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="21">
+        <v>102</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="D5" s="21">
+        <v>3</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="21">
+        <v>103</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="21">
+        <v>3</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="21">
+        <v>104</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D7" s="21">
+        <v>3</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="21">
+        <v>120</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" s="21">
+        <v>3</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="21">
+        <v>121</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D9" s="21">
+        <v>3</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="21">
+        <v>122</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="D10" s="21">
+        <v>3</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="21">
+        <v>123</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="21">
+        <v>3</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="21">
+        <v>124</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="21">
+        <v>3</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="21">
+        <v>127</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" s="21">
+        <v>4</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="21">
+        <v>130</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="21">
+        <v>2</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="21">
+        <v>131</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="21">
+        <v>2</v>
+      </c>
+      <c r="E15" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="21">
+        <v>132</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D16" s="21">
+        <v>2</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="21">
+        <v>133</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="21">
+        <v>2</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" s="21">
+        <v>135</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="D18" s="21">
+        <v>2</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B19" s="21">
+        <v>136</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="21">
+        <v>2</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B20" s="21">
+        <v>137</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="D20" s="21">
+        <v>2</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="21">
+        <v>138</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="21">
+        <v>4</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="21">
+        <v>141</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="D22" s="21">
+        <v>4</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="21">
+        <v>142</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="D23" s="21">
+        <v>4</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="21">
+        <v>143</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="21">
+        <v>3</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B25" s="21">
+        <v>144</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="D25" s="21">
+        <v>3</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B26" s="21">
+        <v>145</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="D26" s="21">
+        <v>3</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="21">
+        <v>146</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="21">
+        <v>3</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="21">
+        <v>147</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="D28" s="21">
+        <v>3</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="21">
+        <v>148</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D29" s="21">
+        <v>3</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="21">
+        <v>149</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="21">
+        <v>3</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="21">
+        <v>150</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D31" s="21">
+        <v>3</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="21">
+        <v>151</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D32" s="21">
+        <v>3</v>
+      </c>
+      <c r="E32" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B33" s="21">
+        <v>152</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="21">
+        <v>3</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B34" s="21">
+        <v>153</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D34" s="21">
+        <v>3</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B35" s="21">
+        <v>154</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="21">
+        <v>3</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="21">
+        <v>155</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D36" s="21">
+        <v>3</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="21">
+        <v>156</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="D37" s="21">
+        <v>3</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="21">
+        <v>157</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="21">
+        <v>3</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="21">
+        <v>160</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D39" s="21">
+        <v>3</v>
+      </c>
+      <c r="E39" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="21">
+        <v>161</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="D40" s="21">
+        <v>3</v>
+      </c>
+      <c r="E40" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B41" s="21">
+        <v>162</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D41" s="21">
+        <v>3</v>
+      </c>
+      <c r="E41" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" s="21">
+        <v>163</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="D42" s="21">
+        <v>3</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B43" s="21">
+        <v>164</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D43" s="21">
+        <v>3</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="21">
+        <v>165</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="D44" s="21">
+        <v>3</v>
+      </c>
+      <c r="E44" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B45" s="21">
+        <v>166</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="D45" s="21">
+        <v>3</v>
+      </c>
+      <c r="E45" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B46" s="21">
+        <v>168</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="D46" s="21">
+        <v>2</v>
+      </c>
+      <c r="E46" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="21">
+        <v>169</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="D47" s="21">
+        <v>2</v>
+      </c>
+      <c r="E47" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B48" s="21">
+        <v>170</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="21">
+        <v>2</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B49" s="21">
+        <v>171</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="D49" s="21">
+        <v>3</v>
+      </c>
+      <c r="E49" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="21">
+        <v>172</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="21">
+        <v>2</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="21">
+        <v>173</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D51" s="21">
+        <v>1</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B52" s="21">
+        <v>174</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="D52" s="21">
+        <v>1</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B53" s="21">
+        <v>175</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="D53" s="21">
+        <v>1</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="15">
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B3" xr:uid="{F41108C8-FC7C-4A9E-B699-1A0CC21F7BCE}">
+      <formula1>"ID"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="C3" xr:uid="{57B90B8A-C4F8-425D-9208-6FC54C2EC2F8}">
+      <formula1>"Title"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="D3" xr:uid="{B8AD3FA3-3F75-4322-B8E1-0680646B4A05}">
+      <formula1>"Priority"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="E3" xr:uid="{786619CA-5E54-45F0-9C11-CE234156DDBA}">
+      <formula1>"State"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="F3" xr:uid="{71B0BD44-F93E-4DE0-A5AE-BDA83F15D940}">
+      <formula1>"Tags"</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B49" xr:uid="{2EE09A0E-5A0A-4859-BAB1-CD4EF4C1796F}">
+      <formula1>"171"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" showInputMessage="1" sqref="C49" xr:uid="{4A37B936-B978-4F6A-84C1-2EFAE7806947}">
+      <formula1>1</formula1>
+      <formula2>255</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="D49" xr:uid="{8B3784E5-8053-425D-8F88-F6A8B0CC84D3}">
+      <formula1>VSTS_ValidationRange_95ca9878f00e4227b038a1809a43bae8</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="E49" xr:uid="{AC576ABE-7CE8-4418-A4DF-81C92B500587}">
+      <formula1>VSTS_ValidationRange_a412f5777bdd44dca0165d52a5a9165a</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" sqref="F49" xr:uid="{D0042F28-E5C4-4CB4-9E9B-D146CF687E4F}">
+      <formula1>0</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showDropDown="1" showInputMessage="1" showErrorMessage="1" errorTitle="Columna de solo lectura" error="TF84013: No puede modificar un campo que sea de solo lectura o un elemento de trabajo que restrinja las actualizaciones de usuarios válidos según los permisos actuales." prompt="Solo lectura" sqref="B45" xr:uid="{F92048E8-565C-4DC4-AC15-CD6F39A3FA50}">
+      <formula1>"166"</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" showInputMessage="1" sqref="C45" xr:uid="{89DF8712-88A5-41B9-950A-974C55598CC9}">
+      <formula1>1</formula1>
+      <formula2>255</formula2>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="D45" xr:uid="{6EDE91F2-CD44-43AC-B1EC-05F0B1F10F3E}">
+      <formula1>VSTS_ValidationRange_95ca9878f00e4227b038a1809a43bae8</formula1>
+    </dataValidation>
+    <dataValidation type="list" operator="equal" showInputMessage="1" showErrorMessage="1" errorTitle="Microsoft Excel" error="TF84042: El valor especificado no se admite en este campo. Seleccione un valor admitido de la lista." sqref="E45" xr:uid="{6DECAD8A-FC95-4FA8-91F7-5FF52E0ED8E4}">
+      <formula1>VSTS_ValidationRange_a412f5777bdd44dca0165d52a5a9165a</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" allowBlank="1" showInputMessage="1" sqref="F45" xr:uid="{943059FC-E798-4444-B6A5-77B89C2F6C01}">
+      <formula1>0</formula1>
+      <formula2>32767</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B054A505-8E3E-4014-A470-9A9FE341BC0A}">
+  <dimension ref="B1:J12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="H2" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+      <c r="I3" s="30">
+        <v>40</v>
+      </c>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="28">
+        <f>COUNTIF('Test Cases System Racing Man.'!D4:D265,1)</f>
+        <v>3</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="30">
+        <f>C4*I3</f>
+        <v>120</v>
+      </c>
+      <c r="F4" s="31"/>
+      <c r="H4" s="14">
+        <v>2</v>
+      </c>
+      <c r="I4" s="30">
+        <v>30</v>
+      </c>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C5" s="28">
+        <f>COUNTIF('Test Cases System Racing Man.'!D5:D266,2)</f>
+        <v>11</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30">
+        <f>C5*I4</f>
+        <v>330</v>
+      </c>
+      <c r="F5" s="31"/>
+      <c r="H5" s="14">
+        <v>3</v>
+      </c>
+      <c r="I5" s="30">
+        <v>15</v>
+      </c>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" s="28">
+        <f>COUNTIF('Test Cases System Racing Man.'!D6:D267,3)</f>
+        <v>30</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30">
+        <f>C6*I5</f>
+        <v>450</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="H6" s="15">
+        <v>4</v>
+      </c>
+      <c r="I6" s="40">
+        <v>5</v>
+      </c>
+      <c r="J6" s="41"/>
+    </row>
+    <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" s="28">
+        <f>COUNTIF('Test Cases System Racing Man.'!D7:D268,4)</f>
+        <v>4</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="40">
+        <f>C7*I6</f>
+        <v>20</v>
+      </c>
+      <c r="F7" s="41"/>
+    </row>
+    <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="42"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="45">
+        <f>SUM(C4:C7)</f>
+        <v>48</v>
+      </c>
+      <c r="D9" s="45"/>
+      <c r="E9" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F9" s="10">
+        <f>SUM(E4:F7)</f>
+        <v>920</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C10" s="32">
+        <f>F9/60</f>
+        <v>15.333333333333334</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C11" s="35">
+        <f>C10/F10</f>
+        <v>3.0666666666666669</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="E11" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="50"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="7">
+        <f>F11*F10</f>
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:D12"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988068B0-9C0A-46E3-9137-06458463F3E1}">
   <dimension ref="A1:AT12"/>
   <sheetViews>
@@ -2702,74 +4192,137 @@
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="51" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="2">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="2">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="2">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="2">
+        <v>1</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U1" s="2">
+        <v>1</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2">
+        <v>1</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="Z1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="2">
-        <v>1</v>
-      </c>
-      <c r="AC1" s="2">
-        <v>1</v>
+      <c r="AB1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>22</v>
+        <v>80</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AF1" s="2">
-        <v>1</v>
+        <v>80</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH1" s="2">
-        <v>1</v>
+        <v>78</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ1" s="2">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="AL1" s="2">
         <v>1</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>79</v>
+      <c r="AM1" s="2">
+        <v>1</v>
       </c>
       <c r="AN1" s="2">
         <v>1</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>81</v>
+      <c r="AO1" s="2">
+        <v>1</v>
       </c>
       <c r="AP1" s="2">
         <v>1</v>
       </c>
-      <c r="AQ1" s="1" t="s">
-        <v>22</v>
+      <c r="AQ1" s="2">
+        <v>1</v>
       </c>
       <c r="AR1" s="2">
         <v>1</v>
       </c>
-      <c r="AS1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>94</v>
+      <c r="AS1" s="2">
+        <v>1</v>
+      </c>
+      <c r="AT1" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
@@ -2785,301 +4338,577 @@
       <c r="D2" t="s">
         <v>8</v>
       </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="K2" s="2">
+        <v>2</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" s="2">
+        <v>2</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O2" s="2">
+        <v>2</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>2</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="S2" s="2">
+        <v>2</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="U2" s="2">
+        <v>2</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="2">
+        <v>2</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="Z2" t="s">
-        <v>10</v>
+        <v>143</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>2</v>
+        <v>128</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>2</v>
+        <v>84</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>2</v>
+        <v>79</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>2</v>
+        <v>72</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>94</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="AL2" s="2">
         <v>2</v>
       </c>
-      <c r="AM2" s="1" t="s">
-        <v>80</v>
+      <c r="AM2" s="2">
+        <v>2</v>
       </c>
       <c r="AN2" s="2">
         <v>2</v>
       </c>
-      <c r="AO2" s="1" t="s">
-        <v>85</v>
+      <c r="AO2" s="2">
+        <v>2</v>
       </c>
       <c r="AP2" s="2">
         <v>2</v>
       </c>
-      <c r="AQ2" s="1" t="s">
-        <v>73</v>
+      <c r="AQ2" s="2">
+        <v>2</v>
       </c>
       <c r="AR2" s="2">
         <v>2</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AS2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AT2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="K3" s="2">
+        <v>3</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M3" s="2">
+        <v>3</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O3" s="2">
+        <v>3</v>
+      </c>
+      <c r="P3" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>3</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" s="2">
+        <v>3</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="U3" s="2">
+        <v>3</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W3" s="2">
+        <v>3</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y3" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AA3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AB3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="2">
-        <v>3</v>
+      <c r="AB3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>19</v>
+        <v>81</v>
       </c>
       <c r="AE3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AF3" s="2">
-        <v>3</v>
+      <c r="AF3" t="s">
+        <v>176</v>
       </c>
       <c r="AG3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AH3" s="2">
-        <v>3</v>
-      </c>
       <c r="AI3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AM3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AN3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AO3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AP3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AQ3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AR3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AS3" s="2">
+        <v>3</v>
+      </c>
+      <c r="AT3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4</v>
+      </c>
+      <c r="I4" t="s">
+        <v>101</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AJ3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>89</v>
-      </c>
-      <c r="AL3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AM3" s="1" t="s">
+      <c r="M4" s="2">
+        <v>4</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>4</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AN3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AO3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AP3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AQ3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AR3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AS3" s="1" t="s">
+      <c r="S4" s="2">
+        <v>4</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="U4" s="2">
+        <v>4</v>
+      </c>
+      <c r="V4" t="s">
+        <v>92</v>
+      </c>
+      <c r="W4" s="2">
+        <v>4</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="AT3" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AA4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AB4" s="2">
-        <v>4</v>
-      </c>
-      <c r="AC4" s="2">
-        <v>4</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>102</v>
+      <c r="AB4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD4" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="AE4" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AF4" s="2">
-        <v>4</v>
-      </c>
       <c r="AG4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AH4" s="2">
-        <v>4</v>
-      </c>
-      <c r="AI4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AJ4" s="2">
-        <v>4</v>
+        <v>81</v>
+      </c>
+      <c r="AH4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>179</v>
+      </c>
+      <c r="AJ4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AK4" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="AL4" s="2">
         <v>4</v>
       </c>
-      <c r="AM4" s="1" t="s">
-        <v>82</v>
+      <c r="AM4" s="2">
+        <v>4</v>
       </c>
       <c r="AN4" s="2">
         <v>4</v>
       </c>
-      <c r="AO4" s="1" t="s">
-        <v>91</v>
+      <c r="AO4" s="2">
+        <v>4</v>
       </c>
       <c r="AP4" s="2">
         <v>4</v>
       </c>
-      <c r="AQ4" t="s">
-        <v>93</v>
+      <c r="AQ4" s="2">
+        <v>4</v>
       </c>
       <c r="AR4" s="2">
         <v>4</v>
       </c>
-      <c r="AS4" s="1" t="s">
+      <c r="AS4" s="2">
+        <v>4</v>
+      </c>
+      <c r="AT4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="AT4" s="1" t="s">
+      <c r="K5" t="s">
+        <v>105</v>
+      </c>
+      <c r="L5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" t="s">
+        <v>106</v>
+      </c>
+      <c r="N5" t="s">
+        <v>86</v>
+      </c>
+      <c r="O5" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>108</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" t="s">
+        <v>109</v>
+      </c>
+      <c r="T5" t="s">
+        <v>91</v>
+      </c>
+      <c r="U5" t="s">
+        <v>110</v>
+      </c>
+      <c r="W5" t="s">
+        <v>111</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AA5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" t="s">
-        <v>105</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>104</v>
-      </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>174</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>175</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>178</v>
+      </c>
+      <c r="AJ5" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>183</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>182</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>185</v>
+      </c>
+      <c r="AP5" t="s">
+        <v>186</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>187</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>188</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>189</v>
+      </c>
+      <c r="AT5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" t="s">
         <v>83</v>
       </c>
-      <c r="AF5" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>86</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AL5" t="s">
-        <v>109</v>
-      </c>
-      <c r="AM5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AO5" t="s">
-        <v>92</v>
-      </c>
-      <c r="AP5" t="s">
-        <v>111</v>
-      </c>
-      <c r="AR5" t="s">
-        <v>112</v>
-      </c>
-      <c r="AS5" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AT5" s="1" t="s">
+      <c r="R6" t="s">
+        <v>89</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y6" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="AA6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AB6" t="s">
+        <v>173</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>177</v>
+      </c>
+      <c r="AJ6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="AK6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="AM6" t="s">
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AJ7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>180</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="X9" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="AS6" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AT6" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AA7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AS7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AA8" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS8" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AT8" t="s">
+      <c r="AK9" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="X10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AK10" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="X11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="X12" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AS9" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AS10" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AS11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="AS12" t="s">
-        <v>101</v>
+      <c r="AK12" t="s">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>